<commit_message>
Dokonceni reseni pomoci dynamickeho programovani a namereni casu
</commit_message>
<xml_diff>
--- a/doc/batoh2.xlsx
+++ b/doc/batoh2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="32">
   <si>
     <t>Soubor 4</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Dynamic</t>
+  </si>
+  <si>
+    <t>Aprox</t>
   </si>
 </sst>
 </file>
@@ -512,11 +515,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="77573504"/>
-        <c:axId val="77592064"/>
+        <c:axId val="62635392"/>
+        <c:axId val="62645760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77573504"/>
+        <c:axId val="62635392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,12 +544,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77592064"/>
+        <c:crossAx val="62645760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77592064"/>
+        <c:axId val="62645760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200000"/>
@@ -573,7 +576,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77573504"/>
+        <c:crossAx val="62635392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -586,7 +589,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -820,11 +823,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="77772672"/>
-        <c:axId val="77774848"/>
+        <c:axId val="62543744"/>
+        <c:axId val="62566400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77772672"/>
+        <c:axId val="62543744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,12 +853,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77774848"/>
+        <c:crossAx val="62566400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77774848"/>
+        <c:axId val="62566400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -881,7 +884,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77772672"/>
+        <c:crossAx val="62543744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -894,7 +897,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1253,7 +1256,7 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1287,15 +1290,20 @@
       <c r="E2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="G2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>30</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>25</v>
@@ -1315,19 +1323,23 @@
         <v>6492</v>
       </c>
       <c r="E3" s="12">
-        <v>0</v>
+        <v>717</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="13">
-        <f>C3/B3</f>
+        <f t="shared" ref="G3:I9" si="0">C3/$B3</f>
         <v>5.3029999999999999</v>
       </c>
-      <c r="H3" s="14">
-        <f>D3/B3</f>
+      <c r="H3" s="13">
+        <f t="shared" si="0"/>
         <v>6.492</v>
       </c>
-      <c r="I3" s="14">
-        <f>E3/C3</f>
+      <c r="I3" s="13">
+        <f t="shared" si="0"/>
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="J3" s="14">
+        <f>F3/D3</f>
         <v>0</v>
       </c>
       <c r="O3">
@@ -1354,19 +1366,23 @@
         <v>11980</v>
       </c>
       <c r="E4" s="12">
-        <v>0</v>
+        <v>13563</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="13">
-        <f t="shared" ref="G4:G8" si="0">C4/B4</f>
+        <f t="shared" si="0"/>
         <v>30.207000000000001</v>
       </c>
-      <c r="H4" s="14">
-        <f t="shared" ref="H4:I14" si="1">D4/B4</f>
+      <c r="H4" s="13">
+        <f t="shared" si="0"/>
         <v>11.98</v>
       </c>
-      <c r="I4" s="14">
-        <f t="shared" si="1"/>
+      <c r="I4" s="13">
+        <f t="shared" si="0"/>
+        <v>13.563000000000001</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" ref="J4:J7" si="1">F4/D4</f>
         <v>0</v>
       </c>
       <c r="O4">
@@ -1393,18 +1409,22 @@
         <v>20971</v>
       </c>
       <c r="E5" s="12">
-        <v>0</v>
+        <v>41656</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="13">
         <f t="shared" si="0"/>
         <v>1044.902</v>
       </c>
-      <c r="H5" s="14">
-        <f t="shared" si="1"/>
+      <c r="H5" s="13">
+        <f t="shared" si="0"/>
         <v>41.942</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="13">
+        <f t="shared" si="0"/>
+        <v>83.311999999999998</v>
+      </c>
+      <c r="J5" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1432,18 +1452,22 @@
         <v>13835</v>
       </c>
       <c r="E6" s="12">
-        <v>0</v>
+        <v>2531</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="13">
         <f t="shared" si="0"/>
         <v>38004.6</v>
       </c>
-      <c r="H6" s="14">
-        <f t="shared" si="1"/>
+      <c r="H6" s="13">
+        <f t="shared" si="0"/>
         <v>1383.5</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="13">
+        <f t="shared" si="0"/>
+        <v>253.1</v>
+      </c>
+      <c r="J6" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1475,18 +1499,22 @@
         <v>6199</v>
       </c>
       <c r="E7" s="12">
-        <v>0</v>
+        <v>471</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>170461</v>
       </c>
-      <c r="H7" s="14">
-        <f t="shared" si="1"/>
+      <c r="H7" s="13">
+        <f t="shared" si="0"/>
         <v>6199</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="13">
+        <f t="shared" si="0"/>
+        <v>471</v>
+      </c>
+      <c r="J7" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1515,17 +1543,23 @@
       <c r="D8" s="12">
         <v>48639</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="12">
+        <v>607</v>
+      </c>
       <c r="F8" s="12"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="14">
-        <f t="shared" si="1"/>
+      <c r="H8" s="13">
+        <f t="shared" si="0"/>
         <v>48639</v>
       </c>
-      <c r="I8" s="14"/>
+      <c r="I8" s="13">
+        <f t="shared" si="0"/>
+        <v>607</v>
+      </c>
+      <c r="J8" s="14"/>
       <c r="K8">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1555,16 +1589,23 @@
       <c r="D9" s="12">
         <v>204087</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="E9" s="12">
+        <v>765</v>
+      </c>
       <c r="F9" s="12"/>
       <c r="G9" s="13">
-        <v>0</v>
-      </c>
-      <c r="H9" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="13">
+        <f t="shared" si="0"/>
         <v>204087</v>
       </c>
-      <c r="I9" s="14"/>
+      <c r="I9" s="13">
+        <f t="shared" si="0"/>
+        <v>765</v>
+      </c>
+      <c r="J9" s="14"/>
       <c r="K9">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1583,11 +1624,17 @@
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+      <c r="E10" s="12">
+        <v>1117</v>
+      </c>
       <c r="F10" s="12"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13">
+        <f>E10/$B10</f>
+        <v>1117</v>
+      </c>
+      <c r="J10" s="14"/>
       <c r="K10">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1602,11 +1649,17 @@
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
+      <c r="E11" s="12">
+        <v>1579</v>
+      </c>
       <c r="F11" s="12"/>
       <c r="G11" s="13"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13">
+        <f>E11/$B11</f>
+        <v>1579</v>
+      </c>
+      <c r="J11" s="14"/>
       <c r="K11">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1621,11 +1674,17 @@
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
+      <c r="E12" s="12">
+        <v>2181</v>
+      </c>
       <c r="F12" s="12"/>
       <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13">
+        <f>E12/$B12</f>
+        <v>2181</v>
+      </c>
+      <c r="J12" s="14"/>
       <c r="K12">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1640,11 +1699,17 @@
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
+      <c r="E13" s="12">
+        <v>2705</v>
+      </c>
       <c r="F13" s="12"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13">
+        <f>E13/$B13</f>
+        <v>2705</v>
+      </c>
+      <c r="J13" s="14"/>
       <c r="K13">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1659,11 +1724,17 @@
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="E14" s="17">
+        <v>3713</v>
+      </c>
       <c r="F14" s="17"/>
       <c r="G14" s="18"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18">
+        <f>E14/$B14</f>
+        <v>3713</v>
+      </c>
+      <c r="J14" s="19"/>
       <c r="K14">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1820,7 +1891,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>